<commit_message>
wrzucenie reszty wyników do excela
</commit_message>
<xml_diff>
--- a/wae_wyniki.xlsx
+++ b/wae_wyniki.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="22056" windowHeight="9528"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="22056" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>rand / bin</t>
   </si>
@@ -34,6 +34,30 @@
   </si>
   <si>
     <t>best / exp</t>
+  </si>
+  <si>
+    <t>F=0.2</t>
+  </si>
+  <si>
+    <t>F=0.5</t>
+  </si>
+  <si>
+    <t>F=0.8</t>
+  </si>
+  <si>
+    <t>cr=0.2</t>
+  </si>
+  <si>
+    <t>cr=0.5</t>
+  </si>
+  <si>
+    <t>cr=0.8</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -370,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -380,7 +404,12 @@
     <col min="5" max="5" width="19.296875" customWidth="1"/>
     <col min="6" max="6" width="17.69921875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="16.296875" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="16.296875" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1054,24 +1083,1730 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="19.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.296875" customWidth="1"/>
+    <col min="6" max="6" width="16.296875" customWidth="1"/>
+    <col min="7" max="7" width="17.19921875" customWidth="1"/>
+    <col min="10" max="10" width="15.296875" customWidth="1"/>
+    <col min="11" max="11" width="16.8984375" customWidth="1"/>
+    <col min="14" max="14" width="14.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1400</v>
+      </c>
+      <c r="C2">
+        <v>-1397.5340000000001</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>-1400</v>
+      </c>
+      <c r="G2">
+        <v>-1399.9949999999999</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>-1400</v>
+      </c>
+      <c r="K2">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1300</v>
+      </c>
+      <c r="C3">
+        <v>23245.75</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>-1300</v>
+      </c>
+      <c r="G3">
+        <v>-1295.2729999999999</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>-1300</v>
+      </c>
+      <c r="K3">
+        <v>-1300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1200</v>
+      </c>
+      <c r="C4">
+        <v>1116116</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>-1200</v>
+      </c>
+      <c r="G4">
+        <v>-978.06230000000005</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>-1200</v>
+      </c>
+      <c r="K4">
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1100</v>
+      </c>
+      <c r="C5">
+        <v>181164.5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>-1100</v>
+      </c>
+      <c r="G5">
+        <v>-1100</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>-1100</v>
+      </c>
+      <c r="K5">
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1000</v>
+      </c>
+      <c r="C6">
+        <v>-996.7731</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>-1000</v>
+      </c>
+      <c r="G6">
+        <v>-999.99720000000002</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>-1000</v>
+      </c>
+      <c r="K6">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-899.99459999999999</v>
+      </c>
+      <c r="C7">
+        <v>-899.99879999999996</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>-900</v>
+      </c>
+      <c r="G7">
+        <v>-900</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>-900</v>
+      </c>
+      <c r="K7">
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-800</v>
+      </c>
+      <c r="C8">
+        <v>-797.49829999999997</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>-800</v>
+      </c>
+      <c r="G8">
+        <v>-799.98289999999997</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>-800</v>
+      </c>
+      <c r="K8">
+        <v>-800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-700</v>
+      </c>
+      <c r="C9">
+        <v>-691.52210000000002</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>-700</v>
+      </c>
+      <c r="G9">
+        <v>-700</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>-700</v>
+      </c>
+      <c r="K9">
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-600</v>
+      </c>
+      <c r="C10">
+        <v>-599.05939999999998</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>-600</v>
+      </c>
+      <c r="G10">
+        <v>-600</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>-600</v>
+      </c>
+      <c r="K10">
+        <v>-598.90989999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-499.99009999999998</v>
+      </c>
+      <c r="C11">
+        <v>-499.06360000000001</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>-500</v>
+      </c>
+      <c r="G11">
+        <v>-499.89420000000001</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>-499.99259999999998</v>
+      </c>
+      <c r="K11">
+        <v>-499.9522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-400</v>
+      </c>
+      <c r="C12">
+        <v>-399.70830000000001</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>-400</v>
+      </c>
+      <c r="G12">
+        <v>-400</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>-400</v>
+      </c>
+      <c r="K12">
+        <v>-395.78769999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-300</v>
+      </c>
+      <c r="C13">
+        <v>-297.98829999999998</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>-300</v>
+      </c>
+      <c r="G13">
+        <v>-296.08319999999998</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>-300</v>
+      </c>
+      <c r="K13">
+        <v>-296.61610000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-200</v>
+      </c>
+      <c r="C14">
+        <v>-196.45160000000001</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>-200</v>
+      </c>
+      <c r="G14">
+        <v>-196.47909999999999</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>-200</v>
+      </c>
+      <c r="K14">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-100</v>
+      </c>
+      <c r="C15">
+        <v>-99.212819999999994</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>-100</v>
+      </c>
+      <c r="G15">
+        <v>-65.423649999999995</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>-99.375649999999993</v>
+      </c>
+      <c r="K15">
+        <v>-45.017670000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>100.3122</v>
+      </c>
+      <c r="C16">
+        <v>117.81440000000001</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>100.3122</v>
+      </c>
+      <c r="G16">
+        <v>130.4853</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>100.62430000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>200.00069999999999</v>
+      </c>
+      <c r="C17">
+        <v>204.3826</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>200</v>
+      </c>
+      <c r="G17">
+        <v>206.42750000000001</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>200.06700000000001</v>
+      </c>
+      <c r="K17">
+        <v>203.05940000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>300.06259999999997</v>
+      </c>
+      <c r="C18">
+        <v>308.5668</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>302.01960000000003</v>
+      </c>
+      <c r="G18">
+        <v>304.774</v>
+      </c>
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <v>302.01960000000003</v>
+      </c>
+      <c r="K18">
+        <v>302.81509999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>402.03300000000002</v>
+      </c>
+      <c r="C19">
+        <v>407.66669999999999</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>400</v>
+      </c>
+      <c r="G19">
+        <v>404.67840000000001</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19">
+        <v>400.20139999999998</v>
+      </c>
+      <c r="K19">
+        <v>402.82600000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>500.14210000000003</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>500</v>
+      </c>
+      <c r="G20">
+        <v>500.1223</v>
+      </c>
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>500</v>
+      </c>
+      <c r="K20">
+        <v>500.01519999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>600.01940000000002</v>
+      </c>
+      <c r="C21">
+        <v>600.01940000000002</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>600.01940000000002</v>
+      </c>
+      <c r="G21">
+        <v>600.01940000000002</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>600</v>
+      </c>
+      <c r="K21">
+        <v>600.01949999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>700</v>
+      </c>
+      <c r="C22">
+        <v>918.98350000000005</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>700</v>
+      </c>
+      <c r="G22">
+        <v>910.70249999999999</v>
+      </c>
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>700</v>
+      </c>
+      <c r="K22">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>801.6223</v>
+      </c>
+      <c r="C23">
+        <v>865.57069999999999</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>800</v>
+      </c>
+      <c r="G23">
+        <v>851.77750000000003</v>
+      </c>
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>800</v>
+      </c>
+      <c r="K23">
+        <v>922.75530000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>900</v>
+      </c>
+      <c r="C24">
+        <v>1150.7650000000001</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>900</v>
+      </c>
+      <c r="G24">
+        <v>900.11630000000002</v>
+      </c>
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24">
+        <v>900</v>
+      </c>
+      <c r="K24">
+        <v>961.9144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1004.843</v>
+      </c>
+      <c r="C25">
+        <v>1074.374</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <v>1000</v>
+      </c>
+      <c r="K25">
+        <v>1009.897</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1100</v>
+      </c>
+      <c r="C26">
+        <v>1173.856</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>1100</v>
+      </c>
+      <c r="G26">
+        <v>1100.9359999999999</v>
+      </c>
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>1100</v>
+      </c>
+      <c r="K26">
+        <v>1187.672</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1200</v>
+      </c>
+      <c r="C27">
+        <v>1261.403</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>1200</v>
+      </c>
+      <c r="G27">
+        <v>1200</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27">
+        <v>1200</v>
+      </c>
+      <c r="K27">
+        <v>1216.9870000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1410.723</v>
+      </c>
+      <c r="C28">
+        <v>1655.366</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>1400</v>
+      </c>
+      <c r="G28">
+        <v>1630.3320000000001</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>1300</v>
+      </c>
+      <c r="K28">
+        <v>1445.4970000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1406.662</v>
+      </c>
+      <c r="C29">
+        <v>1458.961</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>1400</v>
+      </c>
+      <c r="G29">
+        <v>1507.9659999999999</v>
+      </c>
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29">
+        <v>1400</v>
+      </c>
+      <c r="K29">
+        <v>1506.462</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.19921875" customWidth="1"/>
+    <col min="3" max="3" width="16.296875" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="16.8984375" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1400</v>
+      </c>
+      <c r="C2">
+        <v>-1400</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>-1400</v>
+      </c>
+      <c r="G2">
+        <v>-1400</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>-1400</v>
+      </c>
+      <c r="K2">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1300</v>
+      </c>
+      <c r="C3">
+        <v>-1295.6379999999999</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>-1300</v>
+      </c>
+      <c r="G3">
+        <v>-1298.6990000000001</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>-1300</v>
+      </c>
+      <c r="K3">
+        <v>-1253.4949999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1200</v>
+      </c>
+      <c r="C4">
+        <v>-834.61770000000001</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>-1200</v>
+      </c>
+      <c r="G4">
+        <v>-507.50959999999998</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>-1200</v>
+      </c>
+      <c r="K4">
+        <v>-1005.128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1100</v>
+      </c>
+      <c r="C5">
+        <v>-1097.9880000000001</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>-1100</v>
+      </c>
+      <c r="G5">
+        <v>-1067.6579999999999</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>-1100</v>
+      </c>
+      <c r="K5">
+        <v>-1096.269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1000</v>
+      </c>
+      <c r="C6">
+        <v>-999.9991</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>-1000</v>
+      </c>
+      <c r="G6">
+        <v>-1000</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>-1000</v>
+      </c>
+      <c r="K6">
+        <v>-999.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-900</v>
+      </c>
+      <c r="C7">
+        <v>-900</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>-900</v>
+      </c>
+      <c r="G7">
+        <v>-899.99990000000003</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>-900</v>
+      </c>
+      <c r="K7">
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-800</v>
+      </c>
+      <c r="C8">
+        <v>-799.64329999999995</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>-800</v>
+      </c>
+      <c r="G8">
+        <v>-790.44169999999997</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>-800</v>
+      </c>
+      <c r="K8">
+        <v>-798.16470000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-700</v>
+      </c>
+      <c r="C9">
+        <v>-697.42399999999998</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>-700</v>
+      </c>
+      <c r="G9">
+        <v>-699.72559999999999</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>-700</v>
+      </c>
+      <c r="K9">
+        <v>-699.9502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-600</v>
+      </c>
+      <c r="C10">
+        <v>-599.99210000000005</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>-600</v>
+      </c>
+      <c r="G10">
+        <v>-599.88440000000003</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>-600</v>
+      </c>
+      <c r="K10">
+        <v>-599.92690000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-500</v>
+      </c>
+      <c r="C11">
+        <v>-499.87470000000002</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>-500</v>
+      </c>
+      <c r="G11">
+        <v>-499.88350000000003</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>-500</v>
+      </c>
+      <c r="K11">
+        <v>-499.85270000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-400</v>
+      </c>
+      <c r="C12">
+        <v>-398.76440000000002</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>-400</v>
+      </c>
+      <c r="G12">
+        <v>-397.09820000000002</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>-400</v>
+      </c>
+      <c r="K12">
+        <v>-392.95139999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-300</v>
+      </c>
+      <c r="C13">
+        <v>-300</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>-300</v>
+      </c>
+      <c r="G13">
+        <v>-298.89260000000002</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>-300</v>
+      </c>
+      <c r="K13">
+        <v>-298.91419999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-200</v>
+      </c>
+      <c r="C14">
+        <v>-196.47880000000001</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>-200</v>
+      </c>
+      <c r="G14">
+        <v>-200</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>-200</v>
+      </c>
+      <c r="K14">
+        <v>-196.6559</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-99.687830000000005</v>
+      </c>
+      <c r="C15">
+        <v>-59.899970000000003</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>-99.687830000000005</v>
+      </c>
+      <c r="G15">
+        <v>-70.751230000000007</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>-100</v>
+      </c>
+      <c r="K15">
+        <v>-63.934719999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>100.3122</v>
+      </c>
+      <c r="C16">
+        <v>146.4051</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>100.3122</v>
+      </c>
+      <c r="G16">
+        <v>118.7363</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>112.9297</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>200.0001</v>
+      </c>
+      <c r="C17">
+        <v>207.1146</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>200</v>
+      </c>
+      <c r="G17">
+        <v>207.0848</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>200</v>
+      </c>
+      <c r="K17">
+        <v>207.47059999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>302.01960000000003</v>
+      </c>
+      <c r="C18">
+        <v>303.78070000000002</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>300</v>
+      </c>
+      <c r="G18">
+        <v>304.52010000000001</v>
+      </c>
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <v>302.01960000000003</v>
+      </c>
+      <c r="K18">
+        <v>304.41480000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>402.00209999999998</v>
+      </c>
+      <c r="C19">
+        <v>404.53379999999999</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>400</v>
+      </c>
+      <c r="G19">
+        <v>404.8775</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19">
+        <v>402.00209999999998</v>
+      </c>
+      <c r="K19">
+        <v>404.43700000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>500</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>500</v>
+      </c>
+      <c r="G20">
+        <v>500.06290000000001</v>
+      </c>
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>500</v>
+      </c>
+      <c r="K20">
+        <v>500.0197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>600</v>
+      </c>
+      <c r="C21">
+        <v>600.01949999999999</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>600</v>
+      </c>
+      <c r="G21">
+        <v>600.01949999999999</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>600</v>
+      </c>
+      <c r="K21">
+        <v>600.01940000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>700</v>
+      </c>
+      <c r="C22">
+        <v>903.0204</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>700</v>
+      </c>
+      <c r="G22">
+        <v>703.52359999999999</v>
+      </c>
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>700</v>
+      </c>
+      <c r="K22">
+        <v>700.00229999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>800</v>
+      </c>
+      <c r="C23">
+        <v>841.88239999999996</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>800</v>
+      </c>
+      <c r="G23">
+        <v>856.99279999999999</v>
+      </c>
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>800</v>
+      </c>
+      <c r="K23">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>900</v>
+      </c>
+      <c r="C24">
+        <v>916.61879999999996</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>900</v>
+      </c>
+      <c r="G24">
+        <v>916.13210000000004</v>
+      </c>
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24">
+        <v>900</v>
+      </c>
+      <c r="K24">
+        <v>900.5693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1000</v>
+      </c>
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>1000.009</v>
+      </c>
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <v>1003.147</v>
+      </c>
+      <c r="K25">
+        <v>1007.098</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1100</v>
+      </c>
+      <c r="C26">
+        <v>1204.077</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>1200</v>
+      </c>
+      <c r="G26">
+        <v>1199.7180000000001</v>
+      </c>
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>1100</v>
+      </c>
+      <c r="K26">
+        <v>1205.81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1200.0809999999999</v>
+      </c>
+      <c r="C27">
+        <v>1200.0809999999999</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>1200</v>
+      </c>
+      <c r="G27">
+        <v>1200.3810000000001</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27">
+        <v>1200</v>
+      </c>
+      <c r="K27">
+        <v>1200.296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1400</v>
+      </c>
+      <c r="C28">
+        <v>1425.116</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>1300</v>
+      </c>
+      <c r="G28">
+        <v>1618.0150000000001</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>1400</v>
+      </c>
+      <c r="K28">
+        <v>1635.9259999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1400</v>
+      </c>
+      <c r="C29">
+        <v>1504.1790000000001</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>1400</v>
+      </c>
+      <c r="G29">
+        <v>1504.1389999999999</v>
+      </c>
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29">
+        <v>1400</v>
+      </c>
+      <c r="K29">
+        <v>1505.076</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>